<commit_message>
them du lieu text vao database
</commit_message>
<xml_diff>
--- a/MasterSaveDemo/Database_original.xlsx
+++ b/MasterSaveDemo/Database_original.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\NMCNPM\MasterSaveDemo\MasterSaveDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E5E95E-9921-45EB-BCBC-23DF51E2D4ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F32C0B-5525-482C-90FF-AFDB9C879B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
   </bookViews>
   <sheets>
     <sheet name="LOAITIETKIEM" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="142">
   <si>
     <t>Quản lý nhân sự</t>
   </si>
@@ -262,13 +264,214 @@
   </si>
   <si>
     <t>Trung Nguyễn</t>
+  </si>
+  <si>
+    <t>STK0000006</t>
+  </si>
+  <si>
+    <t>STK0000007</t>
+  </si>
+  <si>
+    <t>STK0000008</t>
+  </si>
+  <si>
+    <t>STK0000009</t>
+  </si>
+  <si>
+    <t>STK0000010</t>
+  </si>
+  <si>
+    <t>STK0000011</t>
+  </si>
+  <si>
+    <t>STK0000012</t>
+  </si>
+  <si>
+    <t>STK0000013</t>
+  </si>
+  <si>
+    <t>STK0000014</t>
+  </si>
+  <si>
+    <t>STK0000015</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>Kết quả tính toán chính thức</t>
+  </si>
+  <si>
+    <t>Nhất</t>
+  </si>
+  <si>
+    <t>Sang Hoàng</t>
+  </si>
+  <si>
+    <t>Trần Văn Tới</t>
+  </si>
+  <si>
+    <t>Võ Văn Cả</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn Song</t>
+  </si>
+  <si>
+    <t>mới rút hôm qua</t>
+  </si>
+  <si>
+    <t>chưa rút từ khi mở sổ</t>
+  </si>
+  <si>
+    <t>tới hạn, chưa rút</t>
+  </si>
+  <si>
+    <t>đã đáo hạn 1 lần, chưa rút</t>
+  </si>
+  <si>
+    <t>Trường Thọ</t>
+  </si>
+  <si>
+    <t>Đức Lâm</t>
+  </si>
+  <si>
+    <t>Hoàng Thư</t>
+  </si>
+  <si>
+    <t>Tuấn Tú</t>
+  </si>
+  <si>
+    <t>STK0000016</t>
+  </si>
+  <si>
+    <t>STK0000017</t>
+  </si>
+  <si>
+    <t>STK0000018</t>
+  </si>
+  <si>
+    <t>chưa đủ số ngày gửi tối thiểu</t>
+  </si>
+  <si>
+    <t>La Quán</t>
+  </si>
+  <si>
+    <t>Trung Khang</t>
+  </si>
+  <si>
+    <t>vừa mới gửi</t>
+  </si>
+  <si>
+    <t>vừa rút trong hôm nay</t>
+  </si>
+  <si>
+    <t>Huy Khánh</t>
+  </si>
+  <si>
+    <t>đã đáo hạn 1 lần, chưa rút, chưa tới ngày đáo hạn lần 2</t>
+  </si>
+  <si>
+    <t>đã đáo hạn 1 lần, chưa rút, đã tới ngày đáo hạn lần 2</t>
+  </si>
+  <si>
+    <t>STK0000019</t>
+  </si>
+  <si>
+    <t>STK0000020</t>
+  </si>
+  <si>
+    <t>STK0000021</t>
+  </si>
+  <si>
+    <t>STK0000022</t>
+  </si>
+  <si>
+    <t>STK0000023</t>
+  </si>
+  <si>
+    <t>STK0000024</t>
+  </si>
+  <si>
+    <t>STK0000025</t>
+  </si>
+  <si>
+    <t>STK0000026</t>
+  </si>
+  <si>
+    <t>STK0000027</t>
+  </si>
+  <si>
+    <t>STK0000028</t>
+  </si>
+  <si>
+    <t>STK0000029</t>
+  </si>
+  <si>
+    <t>STK0000030</t>
+  </si>
+  <si>
+    <t>STK0000031</t>
+  </si>
+  <si>
+    <t>Võ Tàng</t>
+  </si>
+  <si>
+    <t>Trung Nhất</t>
+  </si>
+  <si>
+    <t>Trà</t>
+  </si>
+  <si>
+    <t>Võ Thị Hồng</t>
+  </si>
+  <si>
+    <t>Văn Nhất Quý</t>
+  </si>
+  <si>
+    <t>Vinh Hưng</t>
+  </si>
+  <si>
+    <t>Quốc Hoa</t>
+  </si>
+  <si>
+    <t>Lương Nghĩa</t>
+  </si>
+  <si>
+    <t>Anh Thơ</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Toán</t>
+  </si>
+  <si>
+    <t>Vương Trung</t>
+  </si>
+  <si>
+    <t>Toàn</t>
+  </si>
+  <si>
+    <t>Quốc</t>
+  </si>
+  <si>
+    <t>mới rút hôm qua, giả sử đã rút 500 000</t>
+  </si>
+  <si>
+    <t>không thể rút</t>
+  </si>
+  <si>
+    <t>vừa rút trong hôm nay, giả sử đã rút 100 000</t>
+  </si>
+  <si>
+    <t>đã nhập lãi rồi</t>
+  </si>
+  <si>
+    <t>không nhập lãi hàng loạt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +484,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -303,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -315,6 +524,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,18 +923,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96908E76-F1AB-48E4-94A1-7D29496BFA04}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -759,7 +972,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>56</v>
       </c>
@@ -794,7 +1007,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>68</v>
       </c>
@@ -829,7 +1042,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>71</v>
       </c>
@@ -864,7 +1077,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>73</v>
       </c>
@@ -898,22 +1111,1080 @@
       <c r="K5" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="M5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="3">
+        <v>12000000</v>
+      </c>
+      <c r="F6" s="3">
+        <v>300419750</v>
+      </c>
+      <c r="G6" s="4">
+        <v>43956</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="4">
+        <v>43957</v>
+      </c>
+      <c r="J6" s="3">
+        <v>12000000</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" t="s">
+        <v>93</v>
+      </c>
+      <c r="M6" s="3">
+        <v>12010500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="3">
+        <v>8500000</v>
+      </c>
+      <c r="F7" s="3">
+        <v>300419751</v>
+      </c>
+      <c r="G7" s="5">
+        <v>43963</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J7" s="3">
+        <v>8006493</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" t="s">
+        <v>137</v>
+      </c>
+      <c r="M7" s="3">
+        <v>8006604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="3">
+        <v>50000000</v>
+      </c>
+      <c r="F8" s="3">
+        <v>300419752</v>
+      </c>
+      <c r="G8" s="5">
+        <v>44019</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="4">
+        <v>44020</v>
+      </c>
+      <c r="J8" s="3">
+        <v>50000000</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F9" s="3">
+        <v>300419753</v>
+      </c>
+      <c r="G9" s="5">
+        <v>43929</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="4">
+        <v>44020</v>
+      </c>
+      <c r="J9" s="3">
+        <v>9912500</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" t="s">
+        <v>139</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F10" s="3">
+        <v>300419754</v>
+      </c>
+      <c r="G10" s="5">
+        <v>43929</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5</v>
+      </c>
+      <c r="I10" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J10" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" t="s">
+        <v>94</v>
+      </c>
+      <c r="M10" s="3">
+        <v>10125000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="F11" s="3">
+        <v>300419755</v>
+      </c>
+      <c r="G11" s="5">
+        <v>43930</v>
+      </c>
+      <c r="H11" s="3">
+        <v>5</v>
+      </c>
+      <c r="I11" s="4">
+        <v>44020</v>
+      </c>
+      <c r="J11" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11" t="s">
+        <v>103</v>
+      </c>
+      <c r="M11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F12" s="3">
+        <v>300419756</v>
+      </c>
+      <c r="G12" s="5">
+        <v>43928</v>
+      </c>
+      <c r="H12" s="3">
+        <v>5</v>
+      </c>
+      <c r="I12" s="4">
+        <v>44108</v>
+      </c>
+      <c r="J12" s="3">
+        <v>10125000</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" t="s">
+        <v>95</v>
+      </c>
+      <c r="M12" s="3">
+        <v>10125140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="F13" s="3">
+        <v>300419757</v>
+      </c>
+      <c r="G13" s="5">
+        <v>43929</v>
+      </c>
+      <c r="H13" s="3">
+        <v>5</v>
+      </c>
+      <c r="I13" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J13" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" t="s">
+        <v>94</v>
+      </c>
+      <c r="M13" s="3">
+        <v>15187500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="F14" s="3">
+        <v>300419758</v>
+      </c>
+      <c r="G14" s="5">
+        <v>43839</v>
+      </c>
+      <c r="H14" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I14" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J14" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" t="s">
+        <v>94</v>
+      </c>
+      <c r="M14" s="3">
+        <v>5137500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="3">
+        <v>25000000</v>
+      </c>
+      <c r="F15" s="3">
+        <v>300419759</v>
+      </c>
+      <c r="G15" s="5">
+        <v>43839</v>
+      </c>
+      <c r="H15" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I15" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J15" s="3">
+        <v>25000000</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" t="s">
+        <v>94</v>
+      </c>
+      <c r="M15" s="3">
+        <v>25687500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="3">
+        <v>25000000</v>
+      </c>
+      <c r="F16" s="3">
+        <v>300419760</v>
+      </c>
+      <c r="G16" s="5">
+        <v>43840</v>
+      </c>
+      <c r="H16" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I16" s="4">
+        <v>44020</v>
+      </c>
+      <c r="J16" s="3">
+        <v>25000000</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" t="s">
+        <v>103</v>
+      </c>
+      <c r="M16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="3">
+        <v>25000000</v>
+      </c>
+      <c r="F17" s="3">
+        <v>300419761</v>
+      </c>
+      <c r="G17" s="5">
+        <v>43661</v>
+      </c>
+      <c r="H17" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I17" s="4">
+        <v>44021</v>
+      </c>
+      <c r="J17" s="3">
+        <v>25687500</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17" t="s">
+        <v>109</v>
+      </c>
+      <c r="M17" s="3">
+        <v>25751005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="F18" s="3">
+        <v>300419762</v>
+      </c>
+      <c r="G18" s="5">
+        <v>43659</v>
+      </c>
+      <c r="H18" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I18" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J18" s="3">
+        <v>5137500</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18" t="s">
+        <v>110</v>
+      </c>
+      <c r="M18" s="3">
+        <v>5278781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="3">
+        <v>12000000</v>
+      </c>
+      <c r="F19" s="3">
+        <v>300419763</v>
+      </c>
+      <c r="G19" s="4">
+        <v>43956</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I19" s="4">
+        <v>43957</v>
+      </c>
+      <c r="J19" s="3">
+        <v>12000000</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" t="s">
+        <v>93</v>
+      </c>
+      <c r="M19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="3">
+        <v>8500000</v>
+      </c>
+      <c r="F20" s="3">
+        <v>300419764</v>
+      </c>
+      <c r="G20" s="5">
+        <v>43963</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I20" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J20" s="3">
+        <v>8006493</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L20" t="s">
+        <v>92</v>
+      </c>
+      <c r="M20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="3">
+        <v>50000000</v>
+      </c>
+      <c r="F21" s="3">
+        <v>300419765</v>
+      </c>
+      <c r="G21" s="5">
+        <v>44019</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I21" s="4">
+        <v>44020</v>
+      </c>
+      <c r="J21" s="3">
+        <v>50000000</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L21" t="s">
+        <v>106</v>
+      </c>
+      <c r="M21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F22" s="3">
+        <v>300419766</v>
+      </c>
+      <c r="G22" s="5">
+        <v>43929</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I22" s="4">
+        <v>44020</v>
+      </c>
+      <c r="J22" s="3">
+        <v>9912500</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L22" t="s">
+        <v>107</v>
+      </c>
+      <c r="M22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F23" s="3">
+        <v>300419767</v>
+      </c>
+      <c r="G23" s="5">
+        <v>43929</v>
+      </c>
+      <c r="H23" s="3">
+        <v>5</v>
+      </c>
+      <c r="I23" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J23" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L23" t="s">
+        <v>94</v>
+      </c>
+      <c r="M23" s="3">
+        <v>10125000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="F24" s="3">
+        <v>300419768</v>
+      </c>
+      <c r="G24" s="5">
+        <v>43930</v>
+      </c>
+      <c r="H24" s="3">
+        <v>5</v>
+      </c>
+      <c r="I24" s="4">
+        <v>44020</v>
+      </c>
+      <c r="J24" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L24" t="s">
+        <v>103</v>
+      </c>
+      <c r="M24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F25" s="3">
+        <v>300419769</v>
+      </c>
+      <c r="G25" s="5">
+        <v>43928</v>
+      </c>
+      <c r="H25" s="3">
+        <v>5</v>
+      </c>
+      <c r="I25" s="4">
+        <v>44108</v>
+      </c>
+      <c r="J25" s="3">
+        <v>10125000</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L25" t="s">
+        <v>95</v>
+      </c>
+      <c r="M25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="F26" s="3">
+        <v>300419770</v>
+      </c>
+      <c r="G26" s="5">
+        <v>43929</v>
+      </c>
+      <c r="H26" s="3">
+        <v>5</v>
+      </c>
+      <c r="I26" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J26" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L26" t="s">
+        <v>94</v>
+      </c>
+      <c r="M26" s="3">
+        <v>15187500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="F27" s="3">
+        <v>300419771</v>
+      </c>
+      <c r="G27" s="5">
+        <v>43839</v>
+      </c>
+      <c r="H27" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I27" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J27" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L27" t="s">
+        <v>94</v>
+      </c>
+      <c r="M27" s="3">
+        <v>5137500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="3">
+        <v>25000000</v>
+      </c>
+      <c r="F28" s="3">
+        <v>300419772</v>
+      </c>
+      <c r="G28" s="5">
+        <v>43839</v>
+      </c>
+      <c r="H28" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I28" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J28" s="3">
+        <v>25000000</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L28" t="s">
+        <v>94</v>
+      </c>
+      <c r="M28" s="3">
+        <v>25687500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="3">
+        <v>25000000</v>
+      </c>
+      <c r="F29" s="3">
+        <v>300419773</v>
+      </c>
+      <c r="G29" s="5">
+        <v>43840</v>
+      </c>
+      <c r="H29" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I29" s="4">
+        <v>44020</v>
+      </c>
+      <c r="J29" s="3">
+        <v>25000000</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L29" t="s">
+        <v>103</v>
+      </c>
+      <c r="M29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="3">
+        <v>25000000</v>
+      </c>
+      <c r="F30" s="3">
+        <v>300419774</v>
+      </c>
+      <c r="G30" s="5">
+        <v>43661</v>
+      </c>
+      <c r="H30" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I30" s="4">
+        <v>44021</v>
+      </c>
+      <c r="J30" s="3">
+        <v>25687500</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L30" t="s">
+        <v>109</v>
+      </c>
+      <c r="M30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="F31" s="3">
+        <v>300419775</v>
+      </c>
+      <c r="G31" s="5">
+        <v>43659</v>
+      </c>
+      <c r="H31" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I31" s="4">
+        <v>44019</v>
+      </c>
+      <c r="J31" s="3">
+        <v>5137500</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L31" t="s">
+        <v>110</v>
+      </c>
+      <c r="M31" s="3">
+        <v>5278781</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1356,7 +2627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37225493-D1D8-4637-A3DD-25B32AA2FDE3}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix Trung bug: BaoCaoMoDong_ViewModel, Tien: ThayDoiQuyDinh_ViewModel Set input (only number)
</commit_message>
<xml_diff>
--- a/MasterSaveDemo/Database_original.xlsx
+++ b/MasterSaveDemo/Database_original.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lehoa\Dropbox\My Code\codelearns\wpf\MasterSaveDemo\MasterSaveDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2393D85-6B82-4E1B-B399-81A17ADD2287}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6EAE48-738E-4C3D-966A-DD1056FF5112}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
   </bookViews>
   <sheets>
     <sheet name="LOAITIETKIEM" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="145">
   <si>
     <t>Quản lý nhân sự</t>
   </si>
@@ -463,6 +463,15 @@
   </si>
   <si>
     <t>Đóng sổ tự động</t>
+  </si>
+  <si>
+    <t>Có</t>
+  </si>
+  <si>
+    <t>Rút nhỏ hơn hoặc bằng</t>
+  </si>
+  <si>
+    <t>Rút hết</t>
   </si>
 </sst>
 </file>
@@ -510,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -523,6 +532,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,12 +852,15 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
@@ -861,11 +876,11 @@
       <c r="E1" s="3">
         <v>15</v>
       </c>
-      <c r="F1" s="3">
-        <v>0</v>
-      </c>
-      <c r="G1" s="3">
-        <v>1</v>
+      <c r="F1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -884,11 +899,11 @@
       <c r="E2" s="3">
         <v>90</v>
       </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1</v>
+      <c r="F2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -907,11 +922,11 @@
       <c r="E3" s="3">
         <v>180</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
+      <c r="F3" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -923,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96908E76-F1AB-48E4-94A1-7D29496BFA04}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="A1:M31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +966,7 @@
       <c r="E1" s="3">
         <v>4500000</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="6">
         <v>123456789</v>
       </c>
       <c r="G1" s="4">
@@ -986,7 +1001,7 @@
       <c r="E2" s="3">
         <v>123456000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="6">
         <v>152346369</v>
       </c>
       <c r="G2" s="4">
@@ -1021,8 +1036,8 @@
       <c r="E3" s="3">
         <v>2300000</v>
       </c>
-      <c r="F3" s="3">
-        <v>464345364589</v>
+      <c r="F3" s="6">
+        <v>15234634649</v>
       </c>
       <c r="G3" s="4">
         <v>43922</v>
@@ -1056,7 +1071,7 @@
       <c r="E4" s="3">
         <v>1000000</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>345671236</v>
       </c>
       <c r="G4" s="4">
@@ -1091,7 +1106,7 @@
       <c r="E5" s="3">
         <v>12535000</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="6">
         <v>344565467</v>
       </c>
       <c r="G5" s="4">
@@ -1129,7 +1144,7 @@
       <c r="E6" s="3">
         <v>12000000</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>300419750</v>
       </c>
       <c r="G6" s="4">
@@ -1170,7 +1185,7 @@
       <c r="E7" s="3">
         <v>8500000</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <v>300419751</v>
       </c>
       <c r="G7" s="5">
@@ -1211,7 +1226,7 @@
       <c r="E8" s="3">
         <v>50000000</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
         <v>300419752</v>
       </c>
       <c r="G8" s="5">
@@ -1252,7 +1267,7 @@
       <c r="E9" s="3">
         <v>10000000</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="6">
         <v>300419753</v>
       </c>
       <c r="G9" s="5">
@@ -1293,7 +1308,7 @@
       <c r="E10" s="3">
         <v>10000000</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="6">
         <v>300419754</v>
       </c>
       <c r="G10" s="5">
@@ -1334,7 +1349,7 @@
       <c r="E11" s="3">
         <v>15000000</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
         <v>300419755</v>
       </c>
       <c r="G11" s="5">
@@ -1375,7 +1390,7 @@
       <c r="E12" s="3">
         <v>10000000</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="6">
         <v>300419756</v>
       </c>
       <c r="G12" s="5">
@@ -1416,7 +1431,7 @@
       <c r="E13" s="3">
         <v>15000000</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="6">
         <v>300419757</v>
       </c>
       <c r="G13" s="5">
@@ -1457,7 +1472,7 @@
       <c r="E14" s="3">
         <v>5000000</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="6">
         <v>300419758</v>
       </c>
       <c r="G14" s="5">
@@ -1498,7 +1513,7 @@
       <c r="E15" s="3">
         <v>25000000</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="6">
         <v>300419759</v>
       </c>
       <c r="G15" s="5">
@@ -1539,7 +1554,7 @@
       <c r="E16" s="3">
         <v>25000000</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="6">
         <v>300419760</v>
       </c>
       <c r="G16" s="5">
@@ -1580,7 +1595,7 @@
       <c r="E17" s="3">
         <v>25000000</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="6">
         <v>300419761</v>
       </c>
       <c r="G17" s="5">
@@ -1621,7 +1636,7 @@
       <c r="E18" s="3">
         <v>5000000</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="6">
         <v>300419762</v>
       </c>
       <c r="G18" s="5">
@@ -1662,7 +1677,7 @@
       <c r="E19" s="3">
         <v>12000000</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="6">
         <v>300419763</v>
       </c>
       <c r="G19" s="4">
@@ -1703,7 +1718,7 @@
       <c r="E20" s="3">
         <v>8500000</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="6">
         <v>300419764</v>
       </c>
       <c r="G20" s="5">
@@ -1744,7 +1759,7 @@
       <c r="E21" s="3">
         <v>50000000</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="6">
         <v>300419765</v>
       </c>
       <c r="G21" s="5">
@@ -1785,7 +1800,7 @@
       <c r="E22" s="3">
         <v>10000000</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="6">
         <v>300419766</v>
       </c>
       <c r="G22" s="5">
@@ -1826,7 +1841,7 @@
       <c r="E23" s="3">
         <v>10000000</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="6">
         <v>300419767</v>
       </c>
       <c r="G23" s="5">
@@ -1867,7 +1882,7 @@
       <c r="E24" s="3">
         <v>15000000</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="6">
         <v>300419768</v>
       </c>
       <c r="G24" s="5">
@@ -1908,7 +1923,7 @@
       <c r="E25" s="3">
         <v>10000000</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="6">
         <v>300419769</v>
       </c>
       <c r="G25" s="5">
@@ -1949,7 +1964,7 @@
       <c r="E26" s="3">
         <v>15000000</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="6">
         <v>300419770</v>
       </c>
       <c r="G26" s="5">
@@ -1990,7 +2005,7 @@
       <c r="E27" s="3">
         <v>5000000</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="6">
         <v>300419771</v>
       </c>
       <c r="G27" s="5">
@@ -2031,7 +2046,7 @@
       <c r="E28" s="3">
         <v>25000000</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="6">
         <v>300419772</v>
       </c>
       <c r="G28" s="5">
@@ -2072,7 +2087,7 @@
       <c r="E29" s="3">
         <v>25000000</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="6">
         <v>300419773</v>
       </c>
       <c r="G29" s="5">
@@ -2113,7 +2128,7 @@
       <c r="E30" s="3">
         <v>25000000</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="6">
         <v>300419774</v>
       </c>
       <c r="G30" s="5">
@@ -2154,7 +2169,7 @@
       <c r="E31" s="3">
         <v>5000000</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="6">
         <v>300419775</v>
       </c>
       <c r="G31" s="5">
@@ -2190,7 +2205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C901F8-9E1F-451C-B42C-5AB73AC2B6C6}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2416,7 +2431,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C18"/>
+      <selection sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
thêm database test báo cáo mở đóng tháng 6
</commit_message>
<xml_diff>
--- a/MasterSaveDemo/Database_original.xlsx
+++ b/MasterSaveDemo/Database_original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lehoa\Dropbox\My Code\codelearns\wpf\MasterSaveDemo\MasterSaveDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\NMCNPM\MasterSaveDemo\MasterSaveDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6EAE48-738E-4C3D-966A-DD1056FF5112}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C676BD5-86EA-4D2D-B63B-371DA123158E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
   </bookViews>
   <sheets>
     <sheet name="LOAITIETKIEM" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="179">
   <si>
     <t>Quản lý nhân sự</t>
   </si>
@@ -472,6 +472,108 @@
   </si>
   <si>
     <t>Rút hết</t>
+  </si>
+  <si>
+    <t>STK0000032</t>
+  </si>
+  <si>
+    <t>STK0000033</t>
+  </si>
+  <si>
+    <t>STK0000034</t>
+  </si>
+  <si>
+    <t>STK0000035</t>
+  </si>
+  <si>
+    <t>STK0000036</t>
+  </si>
+  <si>
+    <t>STK0000037</t>
+  </si>
+  <si>
+    <t>STK0000038</t>
+  </si>
+  <si>
+    <t>STK0000039</t>
+  </si>
+  <si>
+    <t>STK0000040</t>
+  </si>
+  <si>
+    <t>Kết</t>
+  </si>
+  <si>
+    <t>Quả</t>
+  </si>
+  <si>
+    <t>Hôm</t>
+  </si>
+  <si>
+    <t>Nay</t>
+  </si>
+  <si>
+    <t>Thành</t>
+  </si>
+  <si>
+    <t>Công</t>
+  </si>
+  <si>
+    <t>Tuyệt</t>
+  </si>
+  <si>
+    <t>Đối</t>
+  </si>
+  <si>
+    <t>Yeah</t>
+  </si>
+  <si>
+    <t>STK0000041</t>
+  </si>
+  <si>
+    <t>STK0000042</t>
+  </si>
+  <si>
+    <t>STK0000043</t>
+  </si>
+  <si>
+    <t>STK0000044</t>
+  </si>
+  <si>
+    <t>STK0000045</t>
+  </si>
+  <si>
+    <t>STK0000046</t>
+  </si>
+  <si>
+    <t>STK0000047</t>
+  </si>
+  <si>
+    <t>STK0000048</t>
+  </si>
+  <si>
+    <t>STK0000049</t>
+  </si>
+  <si>
+    <t>Báo</t>
+  </si>
+  <si>
+    <t>Cáo</t>
+  </si>
+  <si>
+    <t>Cầu</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Mắn</t>
+  </si>
+  <si>
+    <t>Tới</t>
+  </si>
+  <si>
+    <t>Hết</t>
   </si>
 </sst>
 </file>
@@ -860,7 +962,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
@@ -936,21 +1038,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96908E76-F1AB-48E4-94A1-7D29496BFA04}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -2192,6 +2294,474 @@
       </c>
       <c r="M31" s="3">
         <v>5278781</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="5">
+        <v>43990</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="5">
+        <v>43898</v>
+      </c>
+      <c r="H33" s="3">
+        <v>5</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0</v>
+      </c>
+      <c r="K33" s="4">
+        <v>43990</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" s="5">
+        <v>43810</v>
+      </c>
+      <c r="H34" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+      <c r="K34" s="4">
+        <v>43990</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="5">
+        <v>43983</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="4">
+        <v>43917</v>
+      </c>
+      <c r="H36" s="3">
+        <v>5</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+      <c r="K36" s="4">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G37" s="5">
+        <v>43989</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="4">
+        <v>44012</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G38" s="5">
+        <v>43819</v>
+      </c>
+      <c r="H38" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0</v>
+      </c>
+      <c r="K38" s="4">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G39" s="5">
+        <v>43918</v>
+      </c>
+      <c r="H39" s="3">
+        <v>5</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0</v>
+      </c>
+      <c r="K39" s="4">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="5">
+        <v>43889</v>
+      </c>
+      <c r="H40" s="3">
+        <v>5</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0</v>
+      </c>
+      <c r="K40" s="4">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" s="5">
+        <v>43989</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0</v>
+      </c>
+      <c r="K41" s="4">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G42" s="5">
+        <v>43889</v>
+      </c>
+      <c r="H42" s="3">
+        <v>5</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0</v>
+      </c>
+      <c r="K42" s="4">
+        <v>43989</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G43" s="5">
+        <v>43781</v>
+      </c>
+      <c r="H43" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0</v>
+      </c>
+      <c r="K43" s="4">
+        <v>43983</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G44" s="5">
+        <v>43988</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0</v>
+      </c>
+      <c r="K44" s="4">
+        <v>44012</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" s="4">
+        <v>43917</v>
+      </c>
+      <c r="H45" s="3">
+        <v>5</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0</v>
+      </c>
+      <c r="K45" s="4">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G46" s="5">
+        <v>43983</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0</v>
+      </c>
+      <c r="K46" s="4">
+        <v>44012</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47" s="5">
+        <v>43819</v>
+      </c>
+      <c r="H47" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G48" s="5">
+        <v>43918</v>
+      </c>
+      <c r="H48" s="3">
+        <v>5</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0</v>
+      </c>
+      <c r="K48" s="4">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G49" s="5">
+        <v>43889</v>
+      </c>
+      <c r="H49" s="3">
+        <v>5</v>
+      </c>
+      <c r="J49" s="3">
+        <v>0</v>
+      </c>
+      <c r="K49" s="4">
+        <v>44008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
De lai ten CSDL cu
</commit_message>
<xml_diff>
--- a/MasterSaveDemo/Database_original.xlsx
+++ b/MasterSaveDemo/Database_original.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lehoa\Dropbox\My Code\codelearns\wpf\MasterSaveDemo\MasterSaveDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6EAE48-738E-4C3D-966A-DD1056FF5112}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C93723-1AB1-4279-9064-EE0EC181675B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
   </bookViews>
   <sheets>
     <sheet name="LOAITIETKIEM" sheetId="5" r:id="rId1"/>
@@ -852,7 +852,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +860,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96908E76-F1AB-48E4-94A1-7D29496BFA04}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,7 +2205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C901F8-9E1F-451C-B42C-5AB73AC2B6C6}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finish product for sending
</commit_message>
<xml_diff>
--- a/MasterSaveDemo/Database_original.xlsx
+++ b/MasterSaveDemo/Database_original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\NMCNPM\MasterSaveDemo\MasterSaveDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lehoa\Dropbox\My Code\codelearns\wpf\MasterSaveDemo\MasterSaveDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F32C0B-5525-482C-90FF-AFDB9C879B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C93723-1AB1-4279-9064-EE0EC181675B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
   </bookViews>
   <sheets>
     <sheet name="LOAITIETKIEM" sheetId="5" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="145">
   <si>
     <t>Quản lý nhân sự</t>
   </si>
@@ -236,15 +234,6 @@
     <t>Châu</t>
   </si>
   <si>
-    <t>SoTienGuiToiThieu</t>
-  </si>
-  <si>
-    <t>TienGuiThemToiThieu</t>
-  </si>
-  <si>
-    <t>DongSoTuDong</t>
-  </si>
-  <si>
     <t>STK0000003</t>
   </si>
   <si>
@@ -465,6 +454,24 @@
   </si>
   <si>
     <t>không nhập lãi hàng loạt</t>
+  </si>
+  <si>
+    <t>Số tiền gửi tối thiểu</t>
+  </si>
+  <si>
+    <t>Tiền gửi thêm tối thiểu</t>
+  </si>
+  <si>
+    <t>Đóng sổ tự động</t>
+  </si>
+  <si>
+    <t>Có</t>
+  </si>
+  <si>
+    <t>Rút nhỏ hơn hoặc bằng</t>
+  </si>
+  <si>
+    <t>Rút hết</t>
   </si>
 </sst>
 </file>
@@ -512,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -525,6 +532,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,10 +852,13 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -863,11 +876,11 @@
       <c r="E1" s="3">
         <v>15</v>
       </c>
-      <c r="F1" s="3">
-        <v>0</v>
-      </c>
-      <c r="G1" s="3">
-        <v>1</v>
+      <c r="F1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -886,11 +899,11 @@
       <c r="E2" s="3">
         <v>90</v>
       </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1</v>
+      <c r="F2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -909,11 +922,11 @@
       <c r="E3" s="3">
         <v>180</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
+      <c r="F3" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -925,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96908E76-F1AB-48E4-94A1-7D29496BFA04}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +966,7 @@
       <c r="E1" s="3">
         <v>4500000</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="6">
         <v>123456789</v>
       </c>
       <c r="G1" s="4">
@@ -988,7 +1001,7 @@
       <c r="E2" s="3">
         <v>123456000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="6">
         <v>152346369</v>
       </c>
       <c r="G2" s="4">
@@ -1009,22 +1022,22 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" s="3">
         <v>2300000</v>
       </c>
-      <c r="F3" s="3">
-        <v>464345364589</v>
+      <c r="F3" s="6">
+        <v>15234634649</v>
       </c>
       <c r="G3" s="4">
         <v>43922</v>
@@ -1044,21 +1057,21 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E4" s="3">
         <v>1000000</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>345671236</v>
       </c>
       <c r="G4" s="4">
@@ -1077,15 +1090,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>58</v>
@@ -1093,7 +1106,7 @@
       <c r="E5" s="3">
         <v>12535000</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="6">
         <v>344565467</v>
       </c>
       <c r="G5" s="4">
@@ -1112,26 +1125,26 @@
         <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E6" s="3">
         <v>12000000</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>300419750</v>
       </c>
       <c r="G6" s="4">
@@ -1150,7 +1163,7 @@
         <v>52</v>
       </c>
       <c r="L6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M6" s="3">
         <v>12010500</v>
@@ -1158,21 +1171,21 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E7" s="3">
         <v>8500000</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <v>300419751</v>
       </c>
       <c r="G7" s="5">
@@ -1191,7 +1204,7 @@
         <v>52</v>
       </c>
       <c r="L7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="M7" s="3">
         <v>8006604</v>
@@ -1199,21 +1212,21 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E8" s="3">
         <v>50000000</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
         <v>300419752</v>
       </c>
       <c r="G8" s="5">
@@ -1232,29 +1245,29 @@
         <v>52</v>
       </c>
       <c r="L8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E9" s="3">
         <v>10000000</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="6">
         <v>300419753</v>
       </c>
       <c r="G9" s="5">
@@ -1273,29 +1286,29 @@
         <v>52</v>
       </c>
       <c r="L9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E10" s="3">
         <v>10000000</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="6">
         <v>300419754</v>
       </c>
       <c r="G10" s="5">
@@ -1314,7 +1327,7 @@
         <v>52</v>
       </c>
       <c r="L10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M10" s="3">
         <v>10125000</v>
@@ -1322,21 +1335,21 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E11" s="3">
         <v>15000000</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
         <v>300419755</v>
       </c>
       <c r="G11" s="5">
@@ -1355,29 +1368,29 @@
         <v>52</v>
       </c>
       <c r="L11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E12" s="3">
         <v>10000000</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="6">
         <v>300419756</v>
       </c>
       <c r="G12" s="5">
@@ -1396,7 +1409,7 @@
         <v>52</v>
       </c>
       <c r="L12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M12" s="3">
         <v>10125140</v>
@@ -1404,21 +1417,21 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E13" s="3">
         <v>15000000</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="6">
         <v>300419757</v>
       </c>
       <c r="G13" s="5">
@@ -1437,7 +1450,7 @@
         <v>52</v>
       </c>
       <c r="L13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M13" s="3">
         <v>15187500</v>
@@ -1445,21 +1458,21 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E14" s="3">
         <v>5000000</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="6">
         <v>300419758</v>
       </c>
       <c r="G14" s="5">
@@ -1478,7 +1491,7 @@
         <v>52</v>
       </c>
       <c r="L14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M14" s="3">
         <v>5137500</v>
@@ -1486,21 +1499,21 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E15" s="3">
         <v>25000000</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="6">
         <v>300419759</v>
       </c>
       <c r="G15" s="5">
@@ -1519,7 +1532,7 @@
         <v>52</v>
       </c>
       <c r="L15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M15" s="3">
         <v>25687500</v>
@@ -1527,21 +1540,21 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E16" s="3">
         <v>25000000</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="6">
         <v>300419760</v>
       </c>
       <c r="G16" s="5">
@@ -1560,29 +1573,29 @@
         <v>52</v>
       </c>
       <c r="L16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E17" s="3">
         <v>25000000</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="6">
         <v>300419761</v>
       </c>
       <c r="G17" s="5">
@@ -1601,7 +1614,7 @@
         <v>52</v>
       </c>
       <c r="L17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M17" s="3">
         <v>25751005</v>
@@ -1609,21 +1622,21 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E18" s="3">
         <v>5000000</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="6">
         <v>300419762</v>
       </c>
       <c r="G18" s="5">
@@ -1642,7 +1655,7 @@
         <v>52</v>
       </c>
       <c r="L18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M18" s="3">
         <v>5278781</v>
@@ -1650,21 +1663,21 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E19" s="3">
         <v>12000000</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="6">
         <v>300419763</v>
       </c>
       <c r="G19" s="4">
@@ -1683,29 +1696,29 @@
         <v>52</v>
       </c>
       <c r="L19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E20" s="3">
         <v>8500000</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="6">
         <v>300419764</v>
       </c>
       <c r="G20" s="5">
@@ -1724,29 +1737,29 @@
         <v>52</v>
       </c>
       <c r="L20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E21" s="3">
         <v>50000000</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="6">
         <v>300419765</v>
       </c>
       <c r="G21" s="5">
@@ -1765,29 +1778,29 @@
         <v>52</v>
       </c>
       <c r="L21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="M21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E22" s="3">
         <v>10000000</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="6">
         <v>300419766</v>
       </c>
       <c r="G22" s="5">
@@ -1806,29 +1819,29 @@
         <v>52</v>
       </c>
       <c r="L22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M22" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E23" s="3">
         <v>10000000</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="6">
         <v>300419767</v>
       </c>
       <c r="G23" s="5">
@@ -1847,7 +1860,7 @@
         <v>52</v>
       </c>
       <c r="L23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M23" s="3">
         <v>10125000</v>
@@ -1855,21 +1868,21 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E24" s="3">
         <v>15000000</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="6">
         <v>300419768</v>
       </c>
       <c r="G24" s="5">
@@ -1888,29 +1901,29 @@
         <v>52</v>
       </c>
       <c r="L24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E25" s="3">
         <v>10000000</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="6">
         <v>300419769</v>
       </c>
       <c r="G25" s="5">
@@ -1929,29 +1942,29 @@
         <v>52</v>
       </c>
       <c r="L25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E26" s="3">
         <v>15000000</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="6">
         <v>300419770</v>
       </c>
       <c r="G26" s="5">
@@ -1970,7 +1983,7 @@
         <v>52</v>
       </c>
       <c r="L26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M26" s="3">
         <v>15187500</v>
@@ -1978,21 +1991,21 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E27" s="3">
         <v>5000000</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="6">
         <v>300419771</v>
       </c>
       <c r="G27" s="5">
@@ -2011,7 +2024,7 @@
         <v>52</v>
       </c>
       <c r="L27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M27" s="3">
         <v>5137500</v>
@@ -2019,21 +2032,21 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E28" s="3">
         <v>25000000</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="6">
         <v>300419772</v>
       </c>
       <c r="G28" s="5">
@@ -2052,7 +2065,7 @@
         <v>52</v>
       </c>
       <c r="L28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M28" s="3">
         <v>25687500</v>
@@ -2060,21 +2073,21 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E29" s="3">
         <v>25000000</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="6">
         <v>300419773</v>
       </c>
       <c r="G29" s="5">
@@ -2093,29 +2106,29 @@
         <v>52</v>
       </c>
       <c r="L29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E30" s="3">
         <v>25000000</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="6">
         <v>300419774</v>
       </c>
       <c r="G30" s="5">
@@ -2134,29 +2147,29 @@
         <v>52</v>
       </c>
       <c r="L30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E31" s="3">
         <v>5000000</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="6">
         <v>300419775</v>
       </c>
       <c r="G31" s="5">
@@ -2175,7 +2188,7 @@
         <v>52</v>
       </c>
       <c r="L31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M31" s="3">
         <v>5278781</v>
@@ -2190,39 +2203,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C901F8-9E1F-451C-B42C-5AB73AC2B6C6}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="3">
         <v>1000000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="3">
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2409,7 +2431,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C18"/>
+      <selection sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Edit toggle TDQD of Tien and fix money show
</commit_message>
<xml_diff>
--- a/MasterSaveDemo/Database_original.xlsx
+++ b/MasterSaveDemo/Database_original.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lehoa\Dropbox\My Code\codelearns\wpf\MasterSaveDemo\MasterSaveDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C93723-1AB1-4279-9064-EE0EC181675B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04928453-05D9-4EB1-8C0B-217F3CD6A447}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{89B3DFB9-8CD2-41B9-8C42-B954F8B96BD4}"/>
   </bookViews>
   <sheets>
     <sheet name="LOAITIETKIEM" sheetId="5" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="NHOMNGUOIDUNG" sheetId="4" r:id="rId5"/>
     <sheet name="PHANQUYEN" sheetId="3" r:id="rId6"/>
     <sheet name="NGUOIDUNG" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -499,12 +500,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -519,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -535,6 +542,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,7 +870,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96908E76-F1AB-48E4-94A1-7D29496BFA04}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,85 +1228,85 @@
         <v>8006604</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="7">
         <v>50000000</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="8">
         <v>300419752</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="9">
         <v>44019</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="7">
         <v>0.5</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="10">
         <v>44020</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="7">
         <v>50000000</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="7">
         <v>10000000</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="8">
         <v>300419753</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="9">
         <v>43929</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="7">
         <v>0.5</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="10">
         <v>44020</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="7">
         <v>9912500</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="K9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="7" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2205,7 +2223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C901F8-9E1F-451C-B42C-5AB73AC2B6C6}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2430,9 +2448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2545176-A033-4907-9C5D-0F0B2862A39B}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:C18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2650,7 +2666,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2748,4 +2764,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F682F2-84F1-4020-A104-4EADA7A3FA62}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>